<commit_message>
Added some saved parameters
</commit_message>
<xml_diff>
--- a/dataDefinitions.xlsx
+++ b/dataDefinitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspaces\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FDEDA9-1863-4857-9A95-FAEAA58C88E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4D5ED3-61BB-4919-92A3-CA03C4901BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Imaging" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Is it orientation or direction or do we need one for each?</t>
+    Is it orientation or direction or do we need one for each?
+Reply:
+    It is both</t>
       </text>
     </comment>
     <comment ref="D5" authorId="1" shapeId="0" xr:uid="{F3CC5868-E23C-45D2-A6D3-FEAF44D81590}">
@@ -133,7 +135,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Is it orientation or direction or do we need one for each?</t>
+    Is it orientation or direction or do we need one for each?
+Reply:
+    Not sure I understand in this context</t>
       </text>
     </comment>
     <comment ref="D12" authorId="4" shapeId="0" xr:uid="{240BF4D0-C8BE-4866-871F-9F967130B8B7}">
@@ -167,7 +171,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Is it orientation or direction or do we need one for each?</t>
+    Is it orientation or direction or do we need one for each?
+Reply:
+    Not sure I under what it means in this context</t>
       </text>
     </comment>
     <comment ref="D26" authorId="8" shapeId="0" xr:uid="{8A9B1EE8-96F0-4644-8B32-D9A471B3619C}">
@@ -185,7 +191,9 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Should we also save the RF map?
-List parameters</t>
+List parameters
+Reply:
+    We discussed that. I am still not sure. It does save time later. But it is a matrix times 2 and times circle sizes if you want to save for each size</t>
       </text>
     </comment>
     <comment ref="D40" authorId="10" shapeId="0" xr:uid="{BFB11941-4183-4706-8E48-0E98D7879634}">
@@ -193,7 +201,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Is this to explain RF map or single trial responses?</t>
+    Is this to explain RF map or single trial responses?
+Reply:
+    RF map</t>
       </text>
     </comment>
     <comment ref="D41" authorId="11" shapeId="0" xr:uid="{6BA2E1AB-2059-4334-A2C3-39CA49050843}">
@@ -201,7 +211,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Is this to explain RF map or single trial responses?</t>
+    Is this to explain RF map or single trial responses?
+Reply:
+    RF map</t>
       </text>
     </comment>
     <comment ref="D43" authorId="12" shapeId="0" xr:uid="{4E79B79D-607E-436C-A727-CE6D5F00E606}">
@@ -212,12 +224,14 @@
     List parameters</t>
       </text>
     </comment>
-    <comment ref="D45" authorId="13" shapeId="0" xr:uid="{7227379D-DCDF-42AD-8CA1-53DF00F3C290}">
+    <comment ref="D46" authorId="13" shapeId="0" xr:uid="{7227379D-DCDF-42AD-8CA1-53DF00F3C290}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Is the width symmetric around the preferred size? If not, maybe better to save the range (min to max circle size eliciting at least half of the max response)</t>
+    Is the width symmetric around the preferred size? If not, maybe better to save the range (min to max circle size eliciting at least half of the max response)
+Reply:
+    Also added range</t>
       </text>
     </comment>
   </commentList>
@@ -225,7 +239,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="267">
   <si>
     <t>File name</t>
   </si>
@@ -311,18 +325,12 @@
     <t>planes.delay</t>
   </si>
   <si>
-    <t>calcium.planes</t>
-  </si>
-  <si>
     <t>planes.zcorrStack</t>
   </si>
   <si>
     <t>planes.zTrace</t>
   </si>
   <si>
-    <t>rois.zprofiles</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -740,12 +748,6 @@
     <t>p-value for test whether neuron responds to gratings</t>
   </si>
   <si>
-    <t>Fitted parameters for orientation tuning curve</t>
-  </si>
-  <si>
-    <t>Fitted parameters for orientation tuning curve during running (1) or not running (2)</t>
-  </si>
-  <si>
     <t>Explained variance of horizontal line</t>
   </si>
   <si>
@@ -758,15 +760,6 @@
     <t>p-value for test whether tuning curves split by running explain data better than tuning curve for all data</t>
   </si>
   <si>
-    <t>Fitted parameters for temporal frequency tuning curve</t>
-  </si>
-  <si>
-    <t>Fitted parameters for spatial frequency tuning curve</t>
-  </si>
-  <si>
-    <t>Fitted parameters for contrast tuning curve</t>
-  </si>
-  <si>
     <t>circlesResp.bestTime</t>
   </si>
   <si>
@@ -927,6 +920,126 @@
   </si>
   <si>
     <t>Explained variance of Gamma function for black (1) and white (2) cirlces</t>
+  </si>
+  <si>
+    <t>rois.zProfiles</t>
+  </si>
+  <si>
+    <t>Current naming</t>
+  </si>
+  <si>
+    <t>gratings.st</t>
+  </si>
+  <si>
+    <t>start of trial</t>
+  </si>
+  <si>
+    <t>gratings.et</t>
+  </si>
+  <si>
+    <t>end of trial</t>
+  </si>
+  <si>
+    <t>gratings.ori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direction of movement </t>
+  </si>
+  <si>
+    <t>gratings.spatialF</t>
+  </si>
+  <si>
+    <t>gratings.temporalF</t>
+  </si>
+  <si>
+    <t>gratings.contrast</t>
+  </si>
+  <si>
+    <t>sparse.st</t>
+  </si>
+  <si>
+    <t>sparse.et</t>
+  </si>
+  <si>
+    <t>sparse.map</t>
+  </si>
+  <si>
+    <t>double [0,0.5,1]</t>
+  </si>
+  <si>
+    <t>value for each square 0 to 1 (0 black , 1 white)</t>
+  </si>
+  <si>
+    <t>sparseArea.edges</t>
+  </si>
+  <si>
+    <t>retinal.st</t>
+  </si>
+  <si>
+    <t>retinal.et</t>
+  </si>
+  <si>
+    <t>retinal.stim</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>description of stimulus ('Off' - black, 'On' - White, 'Grey' - grey, 'ChirpF' - a full contrast chirp changing frequency, 'ChirpC' - a chirp changing contrast, 'Blue' - blue stim, 'Green'- green stim)</t>
+  </si>
+  <si>
+    <t>circles.st</t>
+  </si>
+  <si>
+    <t>circles.et</t>
+  </si>
+  <si>
+    <t>circles.x</t>
+  </si>
+  <si>
+    <t>position of centre</t>
+  </si>
+  <si>
+    <t>circles.y</t>
+  </si>
+  <si>
+    <t>circles.diameter</t>
+  </si>
+  <si>
+    <t>diameter of circle</t>
+  </si>
+  <si>
+    <t>circles.isWhite</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>1 if circle is white, 0 if black</t>
+  </si>
+  <si>
+    <t>Fitted parameters for orientation tuning curve during not running (1) or  running (2)</t>
+  </si>
+  <si>
+    <t>Fitted parameters for temporal frequency tuning curve:  offset, amplitude, preferred frequency, sigma</t>
+  </si>
+  <si>
+    <t>Fitted parameters for spatial frequency tuning curve:  offset, amplitude, preferred frequency, sigma</t>
+  </si>
+  <si>
+    <t>Fitted parameters for orientation tuning curve: offset, amplitude , Direction index, preferred oreintation, sigma</t>
+  </si>
+  <si>
+    <t>Fitted parameters for contrast tuning curve: offset, gain, c50, n</t>
+  </si>
+  <si>
+    <t>circlesSizeTuning.range</t>
+  </si>
+  <si>
+    <t>nUnits, 100,2</t>
+  </si>
+  <si>
+    <t>a range of stimulus sizes that elicit at least half the maximum response. Rest in nan</t>
   </si>
 </sst>
 </file>
@@ -972,10 +1085,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -993,12 +1107,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1007,6 +1115,11 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1037,11 +1150,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1050,12 +1164,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1076,14 +1189,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1102,6 +1231,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Liad Baruchin" id="{A03BC4B0-5E5C-4E6D-9747-ACD0D6A588F9}" userId="0f4ca98258d4c72d" providerId="Windows Live"/>
   <person displayName="Sylvia Schroeder" id="{0ADF8406-BF5E-4CED-BB87-C903C02D50E7}" userId="e3455f6c0eab7117" providerId="Windows Live"/>
   <person displayName="Sylvia Schroeder" id="{DD2572A2-F949-408A-9E94-F1299C882509}" userId="S::ss2302@sussex.ac.uk::906ec1a8-3d42-4d42-8463-a62b90497b18" providerId="AD"/>
 </personList>
@@ -1425,6 +1555,9 @@
   <threadedComment ref="A5" dT="2023-11-24T17:34:57.30" personId="{0ADF8406-BF5E-4CED-BB87-C903C02D50E7}" id="{EAD461D1-502A-482E-B5AA-4D88F7F86347}">
     <text>Is it orientation or direction or do we need one for each?</text>
   </threadedComment>
+  <threadedComment ref="A5" dT="2023-12-07T09:53:12.44" personId="{A03BC4B0-5E5C-4E6D-9747-ACD0D6A588F9}" id="{40F08DEF-0E80-49E6-9594-243D99587E6C}" parentId="{EAD461D1-502A-482E-B5AA-4D88F7F86347}">
+    <text>It is both</text>
+  </threadedComment>
   <threadedComment ref="D5" dT="2023-11-24T18:00:43.77" personId="{0ADF8406-BF5E-4CED-BB87-C903C02D50E7}" id="{F3CC5868-E23C-45D2-A6D3-FEAF44D81590}">
     <text>List parameters</text>
   </threadedComment>
@@ -1433,6 +1566,9 @@
   </threadedComment>
   <threadedComment ref="A12" dT="2023-11-24T17:34:57.30" personId="{0ADF8406-BF5E-4CED-BB87-C903C02D50E7}" id="{359B4ECC-1534-4AA8-A649-22736B3B2DBF}">
     <text>Is it orientation or direction or do we need one for each?</text>
+  </threadedComment>
+  <threadedComment ref="A12" dT="2023-12-07T10:01:59.82" personId="{A03BC4B0-5E5C-4E6D-9747-ACD0D6A588F9}" id="{D3407A65-A5A8-4751-A982-DC499C7A05CA}" parentId="{359B4ECC-1534-4AA8-A649-22736B3B2DBF}">
+    <text>Not sure I understand in this context</text>
   </threadedComment>
   <threadedComment ref="D12" dT="2023-11-24T18:00:48.02" personId="{0ADF8406-BF5E-4CED-BB87-C903C02D50E7}" id="{240BF4D0-C8BE-4866-871F-9F967130B8B7}">
     <text xml:space="preserve">List parameters
@@ -1448,6 +1584,9 @@
   <threadedComment ref="A26" dT="2023-11-24T17:34:57.30" personId="{0ADF8406-BF5E-4CED-BB87-C903C02D50E7}" id="{BC03141D-979C-4E89-8AD4-82AA771B9094}">
     <text>Is it orientation or direction or do we need one for each?</text>
   </threadedComment>
+  <threadedComment ref="A26" dT="2023-12-07T10:02:14.22" personId="{A03BC4B0-5E5C-4E6D-9747-ACD0D6A588F9}" id="{6ED7A23F-C4A8-4C2F-86AA-5BCED04107AF}" parentId="{BC03141D-979C-4E89-8AD4-82AA771B9094}">
+    <text>Not sure I under what it means in this context</text>
+  </threadedComment>
   <threadedComment ref="D26" dT="2023-11-24T18:00:55.01" personId="{0ADF8406-BF5E-4CED-BB87-C903C02D50E7}" id="{8A9B1EE8-96F0-4644-8B32-D9A471B3619C}">
     <text xml:space="preserve">List parameters
 </text>
@@ -1456,17 +1595,29 @@
     <text>Should we also save the RF map?
 List parameters</text>
   </threadedComment>
+  <threadedComment ref="D37" dT="2023-12-07T10:16:52.22" personId="{A03BC4B0-5E5C-4E6D-9747-ACD0D6A588F9}" id="{E5201E0B-7CF8-4DC3-A412-11125024C487}" parentId="{B0EA968D-0F7D-49BD-AA61-531A7AC089EC}">
+    <text>We discussed that. I am still not sure. It does save time later. But it is a matrix times 2 and times circle sizes if you want to save for each size</text>
+  </threadedComment>
   <threadedComment ref="D40" dT="2023-11-24T18:05:10.46" personId="{0ADF8406-BF5E-4CED-BB87-C903C02D50E7}" id="{BFB11941-4183-4706-8E48-0E98D7879634}">
     <text>Is this to explain RF map or single trial responses?</text>
+  </threadedComment>
+  <threadedComment ref="D40" dT="2023-12-07T10:17:04.95" personId="{A03BC4B0-5E5C-4E6D-9747-ACD0D6A588F9}" id="{0A6CC64D-815A-44A5-BA33-5C95EBB32F27}" parentId="{BFB11941-4183-4706-8E48-0E98D7879634}">
+    <text>RF map</text>
   </threadedComment>
   <threadedComment ref="D41" dT="2023-11-24T18:05:10.46" personId="{0ADF8406-BF5E-4CED-BB87-C903C02D50E7}" id="{6BA2E1AB-2059-4334-A2C3-39CA49050843}">
     <text>Is this to explain RF map or single trial responses?</text>
   </threadedComment>
+  <threadedComment ref="D41" dT="2023-12-07T10:17:13.67" personId="{A03BC4B0-5E5C-4E6D-9747-ACD0D6A588F9}" id="{A6C79A34-311E-4943-A29B-E32FB6DFB32D}" parentId="{6BA2E1AB-2059-4334-A2C3-39CA49050843}">
+    <text>RF map</text>
+  </threadedComment>
   <threadedComment ref="D43" dT="2023-11-24T18:03:05.32" personId="{0ADF8406-BF5E-4CED-BB87-C903C02D50E7}" id="{4E79B79D-607E-436C-A727-CE6D5F00E606}">
     <text>List parameters</text>
   </threadedComment>
-  <threadedComment ref="D45" dT="2023-11-24T18:12:03.68" personId="{0ADF8406-BF5E-4CED-BB87-C903C02D50E7}" id="{7227379D-DCDF-42AD-8CA1-53DF00F3C290}">
+  <threadedComment ref="D46" dT="2023-11-24T18:12:03.68" personId="{0ADF8406-BF5E-4CED-BB87-C903C02D50E7}" id="{7227379D-DCDF-42AD-8CA1-53DF00F3C290}">
     <text>Is the width symmetric around the preferred size? If not, maybe better to save the range (min to max circle size eliciting at least half of the max response)</text>
+  </threadedComment>
+  <threadedComment ref="D46" dT="2023-12-07T10:26:35.97" personId="{A03BC4B0-5E5C-4E6D-9747-ACD0D6A588F9}" id="{00B0129E-D4B8-43CB-995A-229825E46AF9}" parentId="{7227379D-DCDF-42AD-8CA1-53DF00F3C290}">
+    <text>Also added range</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1477,7 +1628,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,17 +1640,17 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1518,8 +1669,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>28</v>
+      <c r="A3" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1558,17 +1709,17 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1624,40 +1775,40 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>31</v>
+      <c r="A14" s="4" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>32</v>
+      <c r="A17" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1687,377 +1838,377 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>56</v>
+      <c r="C10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>39</v>
+      <c r="A11" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="8" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>64</v>
+        <v>53</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="7"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>42</v>
+      <c r="A16" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2084,37 +2235,37 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -2123,7 +2274,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2132,35 +2283,35 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -2169,7 +2320,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2178,7 +2329,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
@@ -2187,7 +2338,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2197,11 +2348,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F47D32-613F-478F-B67D-600975316B20}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2213,63 +2364,63 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2279,61 +2430,61 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2343,102 +2494,376 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="12">
+        <v>4</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="15">
-        <v>4</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="C20" s="14" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>141</v>
+      <c r="C23" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="20">
+        <v>4</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2448,11 +2873,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DAE84D7-1D35-455E-9EAE-38426D5ED717}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2464,536 +2889,550 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D6" s="3" t="s">
+    <row r="10" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>177</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D13" s="8"/>
+        <v>166</v>
+      </c>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D14" s="8"/>
+        <v>162</v>
+      </c>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D15" s="8"/>
+        <v>162</v>
+      </c>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D17" s="8"/>
+        <v>162</v>
+      </c>
+      <c r="D17" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>178</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>179</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B35" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="D46" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed fitting definitions for grating
</commit_message>
<xml_diff>
--- a/dataDefinitions.xlsx
+++ b/dataDefinitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4D5ED3-61BB-4919-92A3-CA03C4901BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6249826-D9C2-4A69-8CAA-0F686188C65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Imaging" sheetId="1" r:id="rId1"/>
@@ -1155,7 +1155,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1193,22 +1193,8 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2593,276 +2579,276 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="1" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="2" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="1" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="1" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C33" s="15">
         <v>4</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="8" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="1" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="1" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="1" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="1" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="1" t="s">
         <v>258</v>
       </c>
     </row>
@@ -2876,8 +2862,8 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3379,17 +3365,17 @@
         <v>223</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="1" t="s">
         <v>266</v>
       </c>
     </row>

</xml_diff>